<commit_message>
modify input data and the mappings
</commit_message>
<xml_diff>
--- a/model-data/all_capacities.xlsx
+++ b/model-data/all_capacities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9bf5eff0e82977d5/Documents/Uni-DESKTOP-D41IPJ3/Internship Aalto/EnergyModel/model-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SpineOptNordic\MESSO\model-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="483" documentId="8_{FE77C99A-068E-4581-8E1B-1A0085C5423B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A579871-5D7D-4B53-BA7B-A56D121A9278}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A836E882-20B4-4B66-B341-4A30233C5E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4470" yWindow="2745" windowWidth="29790" windowHeight="15240" xr2:uid="{1BAD80D3-B61F-4294-A8B7-2B0091A5E784}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{1BAD80D3-B61F-4294-A8B7-2B0091A5E784}"/>
   </bookViews>
   <sheets>
     <sheet name="FIN" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="37">
   <si>
     <t>Production Type</t>
   </si>
@@ -134,6 +133,30 @@
   <si>
     <t>is_active</t>
   </si>
+  <si>
+    <t>Aggregated capacity 2020 [MW]</t>
+  </si>
+  <si>
+    <t>Generation unit capacity 2020 [MW]</t>
+  </si>
+  <si>
+    <t>number_of_units</t>
+  </si>
+  <si>
+    <t>alternative</t>
+  </si>
+  <si>
+    <t>RampBase</t>
+  </si>
+  <si>
+    <t>online_variable_type</t>
+  </si>
+  <si>
+    <t>unit_online_variable_type_integer</t>
+  </si>
+  <si>
+    <t>IntergerVariables</t>
+  </si>
 </sst>
 </file>
 
@@ -168,12 +191,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -236,7 +260,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -532,30 +556,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E20367-8F61-4CFD-AF92-8269AB06E53E}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>25</v>
@@ -563,8 +589,23 @@
       <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -579,8 +620,24 @@
         <f>IF(B2&gt;0,"True","False")</f>
         <v>True</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="2">
+        <f>B2/F2</f>
+        <v>88.571428571428569</v>
+      </c>
+      <c r="F2">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -595,8 +652,24 @@
         <f t="shared" ref="D3:D20" si="0">IF(B3&gt;0,"True","False")</f>
         <v>False</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E21" si="1">B3/F3</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -611,8 +684,24 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -627,8 +716,24 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="2">
+        <f t="shared" si="1"/>
+        <v>108.76470588235294</v>
+      </c>
+      <c r="F5">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -643,8 +748,24 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="2">
+        <f t="shared" si="1"/>
+        <v>270.375</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -659,8 +780,24 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="2">
+        <f t="shared" si="1"/>
+        <v>76.470588235294116</v>
+      </c>
+      <c r="F7">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -675,8 +812,24 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -691,8 +844,24 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="2">
+        <f t="shared" si="1"/>
+        <v>227</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -707,8 +876,24 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -723,8 +908,24 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -739,8 +940,24 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="2">
+        <f t="shared" si="1"/>
+        <v>64.244897959183675</v>
+      </c>
+      <c r="F12">
+        <v>49</v>
+      </c>
+      <c r="G12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -755,8 +972,21 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -771,8 +1001,24 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="2">
+        <f t="shared" si="1"/>
+        <v>558.79999999999995</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -787,8 +1033,21 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="2">
+        <f t="shared" si="1"/>
+        <v>218</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -803,8 +1062,21 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="2">
+        <f t="shared" si="1"/>
+        <v>274</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -819,8 +1091,21 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -835,8 +1120,21 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="2">
+        <f t="shared" si="1"/>
+        <v>54.333333333333336</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -851,8 +1149,21 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -867,40 +1178,70 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="1">
-        <v>17274</v>
-      </c>
+      <c r="E20" s="2">
+        <f>B20/F20</f>
+        <v>2145</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" t="str">
+        <f>$C$1&amp;"_hydro-reservoir"</f>
+        <v>FIN_hydro-reservoir</v>
+      </c>
+      <c r="D21" t="str">
+        <f>IF(B21&gt;0,"True","False")</f>
+        <v>False</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="1">
-        <v>0</v>
-      </c>
-      <c r="C24" t="str">
-        <f>$C$1&amp;"_hydro-reservoir"</f>
-        <v>FIN_hydro-reservoir</v>
-      </c>
-      <c r="D24" t="str">
-        <f>IF(B24&gt;0,"True","False")</f>
-        <v>False</v>
-      </c>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <f>SUM(B2:B21)</f>
+        <v>17274</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -912,10 +1253,10 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -929,7 +1270,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>26</v>
@@ -937,7 +1278,21 @@
       <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -957,7 +1312,22 @@
         <f>IF(B2&gt;0,"True","False")</f>
         <v>False</v>
       </c>
-      <c r="I2" s="1"/>
+      <c r="E2" s="2">
+        <f>B2/F2</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -977,7 +1347,22 @@
         <f t="shared" ref="D3:D20" si="0">IF(B3&gt;0,"True","False")</f>
         <v>False</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E20" si="1">B3/F3</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -997,7 +1382,22 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="I4" s="1"/>
+      <c r="E4" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>36</v>
+      </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -1017,7 +1417,22 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-      <c r="I5" s="1"/>
+      <c r="E5" s="2">
+        <f t="shared" si="1"/>
+        <v>128.4</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
+        <v>36</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -1037,7 +1452,22 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="I6" s="1"/>
+      <c r="E6" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
+        <v>36</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -1057,7 +1487,22 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="E7" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" t="s">
+        <v>36</v>
+      </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -1077,7 +1522,22 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="E8" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" t="s">
+        <v>36</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -1097,7 +1557,22 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="I9" s="1"/>
+      <c r="E9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" t="s">
+        <v>36</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -1117,7 +1592,22 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="I10" s="1"/>
+      <c r="E10" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" t="s">
+        <v>36</v>
+      </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -1137,7 +1627,22 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="I11" s="1"/>
+      <c r="E11" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" t="s">
+        <v>36</v>
+      </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1157,7 +1662,22 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-      <c r="I12" s="1"/>
+      <c r="E12" s="2">
+        <f t="shared" si="1"/>
+        <v>7.1366459627329188</v>
+      </c>
+      <c r="F12">
+        <v>161</v>
+      </c>
+      <c r="G12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" t="s">
+        <v>36</v>
+      </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1177,7 +1697,19 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="I13" s="1"/>
+      <c r="E13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" t="s">
+        <v>36</v>
+      </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -1197,7 +1729,22 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="I14" s="1"/>
+      <c r="E14" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" t="s">
+        <v>36</v>
+      </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1217,7 +1764,19 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="I15" s="1"/>
+      <c r="E15" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" t="s">
+        <v>36</v>
+      </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1237,7 +1796,19 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="I16" s="1"/>
+      <c r="E16" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" t="s">
+        <v>36</v>
+      </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1257,7 +1828,19 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="I17" s="1"/>
+      <c r="E17" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" t="s">
+        <v>36</v>
+      </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1277,7 +1860,19 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="I18" s="1"/>
+      <c r="E18" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" t="s">
+        <v>36</v>
+      </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1297,7 +1892,19 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="I19" s="1"/>
+      <c r="E19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" t="s">
+        <v>36</v>
+      </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1317,45 +1924,80 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-      <c r="I20" s="1"/>
+      <c r="E20" s="2">
+        <f t="shared" si="1"/>
+        <v>3068</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" t="s">
+        <v>36</v>
+      </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="I21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1">
+        <v>28185</v>
+      </c>
+      <c r="C21" t="str">
+        <f>$C$1&amp;"_hydro-reservoir"</f>
+        <v>NOR_hydro-reservoir</v>
+      </c>
+      <c r="D21" t="str">
+        <f>IF(B21&gt;0,"True","False")</f>
+        <v>True</v>
+      </c>
+      <c r="E21" s="2">
+        <f>B21/F21</f>
+        <v>309.72527472527474</v>
+      </c>
+      <c r="F21">
+        <v>91</v>
+      </c>
+      <c r="G21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" t="s">
+        <v>36</v>
+      </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B23" s="1">
+        <f>SUM(B2:B21)</f>
         <v>33044</v>
       </c>
-      <c r="D22" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="1">
-        <v>28185</v>
-      </c>
-      <c r="C24" t="str">
-        <f>$C$1&amp;"_hydro-reservoir"</f>
-        <v>NOR_hydro-reservoir</v>
-      </c>
-      <c r="D24" t="str">
-        <f>IF(B24&gt;0,"True","False")</f>
-        <v>True</v>
-      </c>
-      <c r="I24" s="1"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -1370,10 +2012,10 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -1388,7 +2030,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>27</v>
@@ -1396,7 +2038,21 @@
       <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -1416,7 +2072,22 @@
         <f>IF(B2&gt;0,"True","False")</f>
         <v>False</v>
       </c>
-      <c r="I2" s="1"/>
+      <c r="E2" s="2">
+        <f>B2/F2</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -1436,6 +2107,22 @@
         <f t="shared" ref="D3:D20" si="0">IF(B3&gt;0,"True","False")</f>
         <v>False</v>
       </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E20" si="1">B3/F3</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1452,6 +2139,22 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
+      <c r="E4" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1468,6 +2171,22 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
+      <c r="E5" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1484,6 +2203,22 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
+      <c r="E6" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1500,6 +2235,22 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
+      <c r="E7" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1516,6 +2267,22 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
+      <c r="E8" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1532,6 +2299,22 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
+      <c r="E9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1548,6 +2331,22 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
+      <c r="E10" s="2">
+        <f t="shared" si="1"/>
+        <v>8408</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1564,6 +2363,22 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
+      <c r="E11" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1580,6 +2395,22 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
+      <c r="E12" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1596,6 +2427,19 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
+      <c r="E13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1612,6 +2456,22 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
+      <c r="E14" s="2">
+        <f t="shared" si="1"/>
+        <v>1442.6666666666667</v>
+      </c>
+      <c r="F14">
+        <v>6</v>
+      </c>
+      <c r="G14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1628,6 +2488,19 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
+      <c r="E15" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1644,8 +2517,21 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1660,8 +2546,21 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="2">
+        <f t="shared" si="1"/>
+        <v>411</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1676,8 +2575,21 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1692,8 +2604,21 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -1708,35 +2633,73 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="1">
-        <v>42503</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="E20" s="2">
+        <f t="shared" si="1"/>
+        <v>7300</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B24">
+      <c r="B21">
         <v>16431</v>
       </c>
-      <c r="C24" t="str">
+      <c r="C21" t="str">
         <f>$C$1&amp;"_hydro-reservoir"</f>
         <v>SWE_hydro-reservoir</v>
       </c>
-      <c r="D24" t="str">
-        <f>IF(B24&gt;0,"True","False")</f>
+      <c r="D21" t="str">
+        <f>IF(B21&gt;0,"True","False")</f>
         <v>True</v>
       </c>
+      <c r="E21" s="2">
+        <f>B21/F21</f>
+        <v>469.45714285714286</v>
+      </c>
+      <c r="F21">
+        <v>35</v>
+      </c>
+      <c r="G21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <f>SUM(B2:B21)</f>
+        <v>41206</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1748,10 +2711,10 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -1765,7 +2728,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>24</v>
@@ -1773,7 +2736,21 @@
       <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -1793,7 +2770,22 @@
         <f>IF(B2&gt;0,"True","False")</f>
         <v>True</v>
       </c>
-      <c r="I2" s="1"/>
+      <c r="E2" s="2">
+        <f>B2/F2</f>
+        <v>468</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -1813,7 +2805,22 @@
         <f t="shared" ref="D3:D20" si="0">IF(B3&gt;0,"True","False")</f>
         <v>False</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E20" si="1">B3/F3</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -1833,7 +2840,22 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="I4" s="1"/>
+      <c r="E4" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>36</v>
+      </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -1853,7 +2875,22 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-      <c r="I5" s="1"/>
+      <c r="E5" s="2">
+        <f t="shared" si="1"/>
+        <v>133.76923076923077</v>
+      </c>
+      <c r="F5">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
+        <v>36</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -1873,7 +2910,22 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-      <c r="I6" s="1"/>
+      <c r="E6" s="2">
+        <f t="shared" si="1"/>
+        <v>609.33333333333337</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
+        <v>36</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -1893,7 +2945,22 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="E7" s="2">
+        <f t="shared" si="1"/>
+        <v>336.33333333333331</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" t="s">
+        <v>36</v>
+      </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -1913,7 +2980,22 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="E8" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" t="s">
+        <v>36</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -1933,7 +3015,22 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="I9" s="1"/>
+      <c r="E9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" t="s">
+        <v>36</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -1953,7 +3050,22 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="I10" s="1"/>
+      <c r="E10" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" t="s">
+        <v>36</v>
+      </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -1973,7 +3085,22 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="I11" s="1"/>
+      <c r="E11" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" t="s">
+        <v>36</v>
+      </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1993,7 +3120,22 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-      <c r="I12" s="1"/>
+      <c r="E12" s="2">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" t="s">
+        <v>36</v>
+      </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -2013,7 +3155,19 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="I13" s="1"/>
+      <c r="E13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" t="s">
+        <v>36</v>
+      </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -2033,7 +3187,22 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="I14" s="1"/>
+      <c r="E14" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" t="s">
+        <v>36</v>
+      </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -2053,7 +3222,19 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="I15" s="1"/>
+      <c r="E15" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" t="s">
+        <v>36</v>
+      </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -2073,7 +3254,19 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-      <c r="I16" s="1"/>
+      <c r="E16" s="2">
+        <f t="shared" si="1"/>
+        <v>137</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" t="s">
+        <v>36</v>
+      </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -2093,7 +3286,19 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-      <c r="I17" s="1"/>
+      <c r="E17" s="2">
+        <f t="shared" si="1"/>
+        <v>1013</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" t="s">
+        <v>36</v>
+      </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -2113,7 +3318,19 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-      <c r="I18" s="1"/>
+      <c r="E18" s="2">
+        <f t="shared" si="1"/>
+        <v>54.857142857142854</v>
+      </c>
+      <c r="F18">
+        <v>7</v>
+      </c>
+      <c r="G18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" t="s">
+        <v>36</v>
+      </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -2133,7 +3350,19 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-      <c r="I19" s="1"/>
+      <c r="E19" s="2">
+        <f t="shared" si="1"/>
+        <v>1700</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" t="s">
+        <v>36</v>
+      </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -2153,48 +3382,80 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-      <c r="I20" s="1"/>
+      <c r="E20" s="2">
+        <f t="shared" si="1"/>
+        <v>4402</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" t="s">
+        <v>36</v>
+      </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21" t="str">
+        <f>$C$1&amp;"_hydro-reservoir"</f>
+        <v>DEN_hydro-reservoir</v>
+      </c>
+      <c r="D21" t="str">
+        <f>IF(B21&gt;0,"True","False")</f>
+        <v>False</v>
+      </c>
+      <c r="E21" s="2">
+        <f>B21/F21</f>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" t="s">
+        <v>36</v>
+      </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B23" s="1">
+        <f>SUM(B2:B21)</f>
         <v>15919</v>
       </c>
-      <c r="D22" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="1">
-        <v>0</v>
-      </c>
-      <c r="C24" t="str">
-        <f>$C$1&amp;"_hydro-reservoir"</f>
-        <v>DEN_hydro-reservoir</v>
-      </c>
-      <c r="D24" t="str">
-        <f>IF(B24&gt;0,"True","False")</f>
-        <v>False</v>
-      </c>
-      <c r="I24" s="1"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -2206,27 +3467,27 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34185FE9-ED8F-4A26-B18C-A5B04A819B81}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>23</v>
@@ -2234,8 +3495,23 @@
       <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2251,8 +3527,24 @@
         <f>IF(B2&gt;0,"True","False")</f>
         <v>True</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="2">
+        <f>B2/F2</f>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2268,8 +3560,24 @@
         <f t="shared" ref="D3:D20" si="0">IF(B3&gt;0,"True","False")</f>
         <v>False</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E20" si="1">B3/F3</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2285,8 +3593,24 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="2">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2302,8 +3626,24 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="2">
+        <f t="shared" si="1"/>
+        <v>292.89999999999998</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2319,8 +3659,24 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2336,8 +3692,24 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2353,8 +3725,24 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="2">
+        <f t="shared" si="1"/>
+        <v>656.66666666666663</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2370,8 +3758,24 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2387,8 +3791,24 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2404,8 +3824,24 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="2">
+        <f t="shared" si="1"/>
+        <v>900</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2421,8 +3857,24 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="2">
+        <f t="shared" si="1"/>
+        <v>342.8</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -2438,8 +3890,21 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -2455,8 +3920,24 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -2472,8 +3953,21 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="2">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2489,8 +3983,21 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -2506,8 +4013,21 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="2">
+        <f t="shared" si="1"/>
+        <v>235</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -2523,8 +4043,21 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="2">
+        <f t="shared" si="1"/>
+        <v>13.666666666666666</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -2540,8 +4073,21 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -2557,36 +4103,70 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22">
-        <f>Lithuania!B22+Latvia!B22+Estonia!B22</f>
-        <v>9369</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="E20" s="2">
+        <f t="shared" si="1"/>
+        <v>937</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B24">
-        <f>Lithuania!B13+Latvia!B13+Estonia!B13</f>
-        <v>0</v>
-      </c>
-      <c r="C24" t="str">
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21" t="str">
         <f>$C$1&amp;"_hydro-reservoir"</f>
         <v>BAL_hydro-reservoir</v>
       </c>
-      <c r="D24" t="str">
-        <f>IF(B24&gt;0,"True","False")</f>
-        <v>False</v>
-      </c>
+      <c r="D21" t="str">
+        <f>IF(B21&gt;0,"True","False")</f>
+        <v>False</v>
+      </c>
+      <c r="E21" s="2">
+        <f>B21/F21</f>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <f>SUM(B2:B21)</f>
+        <v>9369</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2598,10 +4178,10 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B22"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
@@ -2799,7 +4379,7 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
@@ -2997,7 +4577,7 @@
       <selection sqref="A1:B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
improve data import workflows
</commit_message>
<xml_diff>
--- a/model-data/all_capacities.xlsx
+++ b/model-data/all_capacities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SpineOptNordic\MESSO\model-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59531B67-950B-41AD-84A3-EA52A5F3D44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9F62AB-E24F-41C9-8BB5-D97BB6964DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{1BAD80D3-B61F-4294-A8B7-2B0091A5E784}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1BAD80D3-B61F-4294-A8B7-2B0091A5E784}"/>
   </bookViews>
   <sheets>
     <sheet name="FIN" sheetId="6" r:id="rId1"/>
@@ -1462,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E20367-8F61-4CFD-AF92-8269AB06E53E}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1550,12 +1550,12 @@
         <v>IntegerVariables</v>
       </c>
       <c r="J2" t="str">
-        <f>IF(H2="unit_online_variable_type_integer","30D","")</f>
-        <v>30D</v>
+        <f>IF(H2="unit_online_variable_type_integer","7D","")</f>
+        <v>7D</v>
       </c>
       <c r="K2" t="str">
-        <f>IF(J2="",J2,"RollingHorizon")</f>
-        <v>RollingHorizon</v>
+        <f>IF(J2="",J2,"RollingFixDispatch")</f>
+        <v>RollingFixDispatch</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1592,11 +1592,11 @@
         <v/>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J21" si="3">IF(H3="unit_online_variable_type_integer","30D","")</f>
+        <f t="shared" ref="J3:J16" si="3">IF(H3="unit_online_variable_type_integer","7D","")</f>
         <v/>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K21" si="4">IF(J3="",J3,"RollingHorizon")</f>
+        <f t="shared" ref="K3:K16" si="4">IF(J3="",J3,"RollingFixDispatch")</f>
         <v/>
       </c>
     </row>
@@ -1677,11 +1677,11 @@
       </c>
       <c r="J5" t="str">
         <f t="shared" si="3"/>
-        <v>30D</v>
+        <v>7D</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
+        <v>RollingFixDispatch</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1719,11 +1719,11 @@
       </c>
       <c r="J6" t="str">
         <f t="shared" si="3"/>
-        <v>30D</v>
+        <v>7D</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
+        <v>RollingFixDispatch</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1761,11 +1761,11 @@
       </c>
       <c r="J7" t="str">
         <f t="shared" si="3"/>
-        <v>30D</v>
+        <v>7D</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
+        <v>RollingFixDispatch</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1845,11 +1845,11 @@
       </c>
       <c r="J9" t="str">
         <f t="shared" si="3"/>
-        <v>30D</v>
+        <v>7D</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
+        <v>RollingFixDispatch</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1927,14 +1927,6 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J11" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K11" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1969,14 +1961,6 @@
         <f t="shared" si="2"/>
         <v>IntegerVariables</v>
       </c>
-      <c r="J12" t="str">
-        <f t="shared" si="3"/>
-        <v>30D</v>
-      </c>
-      <c r="K12" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
-      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -2004,7 +1988,7 @@
         <v>31</v>
       </c>
       <c r="H13" s="7" t="str">
-        <f>IF(D13,"unit_online_variable_type_integer","")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I13" t="str">
@@ -2055,11 +2039,11 @@
       </c>
       <c r="J14" t="str">
         <f t="shared" si="3"/>
-        <v>30D</v>
+        <v>7D</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
+        <v>RollingFixDispatch</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2097,11 +2081,11 @@
       </c>
       <c r="J15" t="str">
         <f t="shared" si="3"/>
-        <v>30D</v>
+        <v>7D</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
+        <v>RollingFixDispatch</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2139,11 +2123,11 @@
       </c>
       <c r="J16" t="str">
         <f t="shared" si="3"/>
-        <v>30D</v>
+        <v>7D</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
+        <v>RollingFixDispatch</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2171,22 +2155,7 @@
       <c r="G17" t="s">
         <v>31</v>
       </c>
-      <c r="H17" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J17" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -2222,12 +2191,12 @@
         <v>IntegerVariables</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" si="3"/>
-        <v>30D</v>
+        <f t="shared" ref="J18" si="6">IF(H18="unit_online_variable_type_integer","7D","")</f>
+        <v>7D</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
+        <f t="shared" ref="K18" si="7">IF(J18="",J18,"RollingFixDispatch")</f>
+        <v>RollingFixDispatch</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -2255,22 +2224,7 @@
       <c r="G19" t="s">
         <v>31</v>
       </c>
-      <c r="H19" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J19" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H19" s="7"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -2297,22 +2251,7 @@
       <c r="G20" t="s">
         <v>31</v>
       </c>
-      <c r="H20" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>unit_online_variable_type_integer</v>
-      </c>
-      <c r="I20" t="str">
-        <f t="shared" si="2"/>
-        <v>IntegerVariables</v>
-      </c>
-      <c r="J20" t="str">
-        <f t="shared" si="3"/>
-        <v>30D</v>
-      </c>
-      <c r="K20" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
-      </c>
+      <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -2345,14 +2284,6 @@
       </c>
       <c r="I21" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J21" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K21" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -2386,7 +2317,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K1048576"/>
+      <selection activeCell="H11" sqref="H11:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2471,11 +2402,11 @@
         <v/>
       </c>
       <c r="J2" t="str">
-        <f>IF(H2="unit_online_variable_type_integer","30D","")</f>
+        <f>IF(H2="unit_online_variable_type_integer","7D","")</f>
         <v/>
       </c>
       <c r="K2" t="str">
-        <f>IF(J2="",J2,"RollingHorizon")</f>
+        <f>IF(J2="",J2,"RollingFixDispatch")</f>
         <v/>
       </c>
       <c r="L2" s="1"/>
@@ -2510,15 +2441,15 @@
         <v/>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I5" si="2">IF(H3="",H3,"IntegerVariables")</f>
+        <f t="shared" ref="I3:I21" si="2">IF(H3="",H3,"IntegerVariables")</f>
         <v/>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J21" si="3">IF(H3="unit_online_variable_type_integer","30D","")</f>
+        <f t="shared" ref="J3:J16" si="3">IF(H3="unit_online_variable_type_integer","7D","")</f>
         <v/>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K21" si="4">IF(J3="",J3,"RollingHorizon")</f>
+        <f t="shared" ref="K3:K16" si="4">IF(J3="",J3,"RollingFixDispatch")</f>
         <v/>
       </c>
       <c r="L3" s="1"/>
@@ -2549,7 +2480,7 @@
         <v>31</v>
       </c>
       <c r="H4" s="7" t="str">
-        <f t="shared" ref="H4:H5" si="5">IF(D4,"unit_online_variable_type_integer","")</f>
+        <f t="shared" ref="H4:H21" si="5">IF(D4,"unit_online_variable_type_integer","")</f>
         <v/>
       </c>
       <c r="I4" t="str">
@@ -2601,11 +2532,11 @@
       </c>
       <c r="J5" t="str">
         <f t="shared" si="3"/>
-        <v>30D</v>
+        <v>7D</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
+        <v>RollingFixDispatch</v>
       </c>
       <c r="L5" s="1"/>
     </row>
@@ -2635,11 +2566,11 @@
         <v>31</v>
       </c>
       <c r="H6" s="7" t="str">
-        <f t="shared" ref="H6:H21" si="6">IF(D6,"unit_online_variable_type_integer","")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I6" t="str">
-        <f t="shared" ref="I6:I21" si="7">IF(H6="",H6,"IntegerVariables")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J6" t="str">
@@ -2678,11 +2609,11 @@
         <v>31</v>
       </c>
       <c r="H7" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J7" t="str">
@@ -2721,11 +2652,11 @@
         <v>31</v>
       </c>
       <c r="H8" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J8" t="str">
@@ -2764,11 +2695,11 @@
         <v>31</v>
       </c>
       <c r="H9" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J9" t="str">
@@ -2807,11 +2738,11 @@
         <v>31</v>
       </c>
       <c r="H10" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J10" t="str">
@@ -2842,20 +2773,12 @@
       </c>
       <c r="E11" s="2"/>
       <c r="H11" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>IntegerVariables</v>
-      </c>
-      <c r="J11" t="str">
-        <f t="shared" si="3"/>
-        <v>30D</v>
-      </c>
-      <c r="K11" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
       </c>
       <c r="L11" s="1"/>
     </row>
@@ -2885,20 +2808,12 @@
         <v>31</v>
       </c>
       <c r="H12" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>IntegerVariables</v>
-      </c>
-      <c r="J12" t="str">
-        <f t="shared" si="3"/>
-        <v>30D</v>
-      </c>
-      <c r="K12" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
       </c>
       <c r="L12" s="1"/>
     </row>
@@ -2928,11 +2843,11 @@
         <v>31</v>
       </c>
       <c r="H13" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J13" t="str">
@@ -2971,11 +2886,11 @@
         <v>31</v>
       </c>
       <c r="H14" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J14" t="str">
@@ -3014,11 +2929,11 @@
         <v>31</v>
       </c>
       <c r="H15" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J15" t="str">
@@ -3057,11 +2972,11 @@
         <v>31</v>
       </c>
       <c r="H16" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J16" t="str">
@@ -3099,22 +3014,7 @@
       <c r="G17" t="s">
         <v>31</v>
       </c>
-      <c r="H17" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I17" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="J17" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H17" s="7"/>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -3143,19 +3043,19 @@
         <v>31</v>
       </c>
       <c r="H18" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I18" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="J18" si="6">IF(H18="unit_online_variable_type_integer","7D","")</f>
         <v/>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="K18" si="7">IF(J18="",J18,"RollingFixDispatch")</f>
         <v/>
       </c>
       <c r="L18" s="1"/>
@@ -3185,22 +3085,7 @@
       <c r="G19" t="s">
         <v>31</v>
       </c>
-      <c r="H19" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I19" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="J19" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H19" s="7"/>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -3228,22 +3113,7 @@
       <c r="G20" t="s">
         <v>31</v>
       </c>
-      <c r="H20" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>unit_online_variable_type_integer</v>
-      </c>
-      <c r="I20" t="str">
-        <f t="shared" si="7"/>
-        <v>IntegerVariables</v>
-      </c>
-      <c r="J20" t="str">
-        <f t="shared" si="3"/>
-        <v>30D</v>
-      </c>
-      <c r="K20" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
-      </c>
+      <c r="H20" s="7"/>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -3272,20 +3142,12 @@
         <v>31</v>
       </c>
       <c r="H21" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I21" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>IntegerVariables</v>
-      </c>
-      <c r="J21" t="str">
-        <f t="shared" si="3"/>
-        <v>30D</v>
-      </c>
-      <c r="K21" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
       </c>
       <c r="L21" s="1"/>
     </row>
@@ -3324,7 +3186,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K1048576"/>
+      <selection activeCell="H11" sqref="H11:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3408,11 +3270,11 @@
         <v/>
       </c>
       <c r="J2" t="str">
-        <f>IF(H2="unit_online_variable_type_integer","30D","")</f>
+        <f>IF(H2="unit_online_variable_type_integer","7D","")</f>
         <v/>
       </c>
       <c r="K2" t="str">
-        <f>IF(J2="",J2,"RollingHorizon")</f>
+        <f>IF(J2="",J2,"RollingFixDispatch")</f>
         <v/>
       </c>
       <c r="L2" s="1"/>
@@ -3451,11 +3313,11 @@
         <v/>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J21" si="3">IF(H3="unit_online_variable_type_integer","30D","")</f>
+        <f t="shared" ref="J3:J16" si="3">IF(H3="unit_online_variable_type_integer","7D","")</f>
         <v/>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K21" si="4">IF(J3="",J3,"RollingHorizon")</f>
+        <f t="shared" ref="K3:K16" si="4">IF(J3="",J3,"RollingFixDispatch")</f>
         <v/>
       </c>
     </row>
@@ -3746,11 +3608,11 @@
       </c>
       <c r="J10" t="str">
         <f t="shared" si="3"/>
-        <v>30D</v>
+        <v>7D</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
+        <v>RollingFixDispatch</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -3778,13 +3640,12 @@
       <c r="G11" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="7"/>
-      <c r="J11" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K11" t="str">
-        <f t="shared" si="4"/>
+      <c r="H11" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3821,14 +3682,6 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="J12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -3856,7 +3709,7 @@
         <v>31</v>
       </c>
       <c r="H13" s="7" t="str">
-        <f>IF(D13,"unit_online_variable_type_integer","")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I13" t="str">
@@ -3907,11 +3760,11 @@
       </c>
       <c r="J14" t="str">
         <f t="shared" si="3"/>
-        <v>30D</v>
+        <v>7D</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
+        <v>RollingFixDispatch</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -4023,22 +3876,7 @@
       <c r="G17" t="s">
         <v>31</v>
       </c>
-      <c r="H17" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>unit_online_variable_type_integer</v>
-      </c>
-      <c r="I17" t="str">
-        <f t="shared" si="2"/>
-        <v>IntegerVariables</v>
-      </c>
-      <c r="J17" t="str">
-        <f t="shared" si="3"/>
-        <v>30D</v>
-      </c>
-      <c r="K17" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
-      </c>
+      <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -4074,11 +3912,11 @@
         <v/>
       </c>
       <c r="J18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="J18" si="6">IF(H18="unit_online_variable_type_integer","7D","")</f>
         <v/>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="K18" si="7">IF(J18="",J18,"RollingFixDispatch")</f>
         <v/>
       </c>
     </row>
@@ -4107,22 +3945,7 @@
       <c r="G19" t="s">
         <v>31</v>
       </c>
-      <c r="H19" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J19" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H19" s="7"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -4149,22 +3972,7 @@
       <c r="G20" t="s">
         <v>31</v>
       </c>
-      <c r="H20" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>unit_online_variable_type_integer</v>
-      </c>
-      <c r="I20" t="str">
-        <f t="shared" si="2"/>
-        <v>IntegerVariables</v>
-      </c>
-      <c r="J20" t="str">
-        <f t="shared" si="3"/>
-        <v>30D</v>
-      </c>
-      <c r="K20" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
-      </c>
+      <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -4198,14 +4006,6 @@
       <c r="I21" t="str">
         <f t="shared" si="2"/>
         <v>IntegerVariables</v>
-      </c>
-      <c r="J21" t="str">
-        <f t="shared" si="3"/>
-        <v>30D</v>
-      </c>
-      <c r="K21" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -4241,7 +4041,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K1048576"/>
+      <selection activeCell="H11" sqref="H11:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4306,7 +4106,7 @@
         <f>IF(B2&gt;0,"True","False")</f>
         <v>True</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="2">
         <f>B2/F2</f>
         <v>424</v>
       </c>
@@ -4325,12 +4125,12 @@
         <v>IntegerVariables</v>
       </c>
       <c r="J2" t="str">
-        <f>IF(H2="unit_online_variable_type_integer","30D","")</f>
-        <v>30D</v>
+        <f>IF(H2="unit_online_variable_type_integer","7D","")</f>
+        <v>7D</v>
       </c>
       <c r="K2" t="str">
-        <f>IF(J2="",J2,"RollingHorizon")</f>
-        <v>RollingHorizon</v>
+        <f>IF(J2="",J2,"RollingFixDispatch")</f>
+        <v>RollingFixDispatch</v>
       </c>
       <c r="L2" s="1"/>
     </row>
@@ -4349,7 +4149,7 @@
         <f t="shared" ref="D3:D20" si="0">IF(B3&gt;0,"True","False")</f>
         <v>False</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="2">
         <f t="shared" ref="E3:E20" si="1">B3/F3</f>
         <v>0</v>
       </c>
@@ -4368,11 +4168,11 @@
         <v/>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J21" si="3">IF(H3="unit_online_variable_type_integer","30D","")</f>
+        <f t="shared" ref="J3:J16" si="3">IF(H3="unit_online_variable_type_integer","7D","")</f>
         <v/>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K21" si="4">IF(J3="",J3,"RollingHorizon")</f>
+        <f t="shared" ref="K3:K16" si="4">IF(J3="",J3,"RollingFixDispatch")</f>
         <v/>
       </c>
       <c r="L3" s="1"/>
@@ -4392,7 +4192,7 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4435,7 +4235,7 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="2">
         <f t="shared" si="1"/>
         <v>140.46153846153845</v>
       </c>
@@ -4455,11 +4255,11 @@
       </c>
       <c r="J5" t="str">
         <f t="shared" si="3"/>
-        <v>30D</v>
+        <v>7D</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
+        <v>RollingFixDispatch</v>
       </c>
       <c r="L5" s="1"/>
     </row>
@@ -4478,7 +4278,7 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="2">
         <f t="shared" si="1"/>
         <v>609.33333333333337</v>
       </c>
@@ -4498,11 +4298,11 @@
       </c>
       <c r="J6" t="str">
         <f t="shared" si="3"/>
-        <v>30D</v>
+        <v>7D</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
+        <v>RollingFixDispatch</v>
       </c>
       <c r="L6" s="1"/>
     </row>
@@ -4521,7 +4321,7 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="2">
         <f t="shared" si="1"/>
         <v>335.66666666666669</v>
       </c>
@@ -4541,11 +4341,11 @@
       </c>
       <c r="J7" t="str">
         <f t="shared" si="3"/>
-        <v>30D</v>
+        <v>7D</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
+        <v>RollingFixDispatch</v>
       </c>
       <c r="L7" s="1"/>
     </row>
@@ -4564,7 +4364,7 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4607,7 +4407,7 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4650,7 +4450,7 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4693,7 +4493,7 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4703,13 +4503,12 @@
       <c r="G11" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="7"/>
-      <c r="J11" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K11" t="str">
-        <f t="shared" si="4"/>
+      <c r="H11" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="L11" s="1"/>
@@ -4729,7 +4528,7 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="2">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -4747,14 +4546,6 @@
         <f t="shared" si="2"/>
         <v>IntegerVariables</v>
       </c>
-      <c r="J12" t="str">
-        <f t="shared" si="3"/>
-        <v>30D</v>
-      </c>
-      <c r="K12" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
-      </c>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -4772,7 +4563,7 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4783,7 +4574,7 @@
         <v>31</v>
       </c>
       <c r="H13" s="7" t="str">
-        <f>IF(D13,"unit_online_variable_type_integer","")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I13" t="str">
@@ -4815,7 +4606,7 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4858,7 +4649,7 @@
         <f t="shared" si="0"/>
         <v>False</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4901,7 +4692,7 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="2">
         <f t="shared" si="1"/>
         <v>146</v>
       </c>
@@ -4921,11 +4712,11 @@
       </c>
       <c r="J16" t="str">
         <f t="shared" si="3"/>
-        <v>30D</v>
+        <v>7D</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
+        <v>RollingFixDispatch</v>
       </c>
       <c r="L16" s="1"/>
     </row>
@@ -4944,7 +4735,7 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="2">
         <f t="shared" si="1"/>
         <v>1002</v>
       </c>
@@ -4954,22 +4745,7 @@
       <c r="G17" t="s">
         <v>31</v>
       </c>
-      <c r="H17" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>unit_online_variable_type_integer</v>
-      </c>
-      <c r="I17" t="str">
-        <f t="shared" si="2"/>
-        <v>IntegerVariables</v>
-      </c>
-      <c r="J17" t="str">
-        <f t="shared" si="3"/>
-        <v>30D</v>
-      </c>
-      <c r="K17" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
-      </c>
+      <c r="H17" s="7"/>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -4987,7 +4763,7 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="2">
         <f t="shared" si="1"/>
         <v>54.857142857142854</v>
       </c>
@@ -5006,12 +4782,12 @@
         <v>IntegerVariables</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" si="3"/>
-        <v>30D</v>
+        <f t="shared" ref="J18" si="6">IF(H18="unit_online_variable_type_integer","7D","")</f>
+        <v>7D</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
+        <f t="shared" ref="K18" si="7">IF(J18="",J18,"RollingFixDispatch")</f>
+        <v>RollingFixDispatch</v>
       </c>
       <c r="L18" s="1"/>
     </row>
@@ -5030,7 +4806,7 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="2">
         <f t="shared" si="1"/>
         <v>1700</v>
       </c>
@@ -5040,22 +4816,7 @@
       <c r="G19" t="s">
         <v>31</v>
       </c>
-      <c r="H19" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>unit_online_variable_type_integer</v>
-      </c>
-      <c r="I19" t="str">
-        <f t="shared" si="2"/>
-        <v>IntegerVariables</v>
-      </c>
-      <c r="J19" t="str">
-        <f t="shared" si="3"/>
-        <v>30D</v>
-      </c>
-      <c r="K19" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
-      </c>
+      <c r="H19" s="7"/>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -5073,7 +4834,7 @@
         <f t="shared" si="0"/>
         <v>True</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="2">
         <f t="shared" si="1"/>
         <v>4423</v>
       </c>
@@ -5083,22 +4844,7 @@
       <c r="G20" t="s">
         <v>31</v>
       </c>
-      <c r="H20" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>unit_online_variable_type_integer</v>
-      </c>
-      <c r="I20" t="str">
-        <f t="shared" si="2"/>
-        <v>IntegerVariables</v>
-      </c>
-      <c r="J20" t="str">
-        <f t="shared" si="3"/>
-        <v>30D</v>
-      </c>
-      <c r="K20" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
-      </c>
+      <c r="H20" s="7"/>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -5116,7 +4862,7 @@
         <f>IF(B21&gt;0,"True","False")</f>
         <v>False</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="2">
         <f>B21/F21</f>
         <v>0</v>
       </c>
@@ -5132,14 +4878,6 @@
       </c>
       <c r="I21" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J21" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K21" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="L21" s="1"/>
@@ -5178,8 +4916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34185FE9-ED8F-4A26-B18C-A5B04A819B81}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5265,12 +5003,12 @@
         <v>IntegerVariables</v>
       </c>
       <c r="J2" t="str">
-        <f>IF(H2="unit_online_variable_type_integer","30D","")</f>
-        <v>30D</v>
+        <f>IF(H2="unit_online_variable_type_integer","7D","")</f>
+        <v>7D</v>
       </c>
       <c r="K2" t="str">
-        <f>IF(J2="",J2,"RollingHorizon")</f>
-        <v>RollingHorizon</v>
+        <f>IF(J2="",J2,"RollingFixDispatch")</f>
+        <v>RollingFixDispatch</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -5308,11 +5046,11 @@
         <v/>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J21" si="3">IF(H3="unit_online_variable_type_integer","30D","")</f>
+        <f t="shared" ref="J3:J16" si="3">IF(H3="unit_online_variable_type_integer","7D","")</f>
         <v/>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K21" si="4">IF(J3="",J3,"RollingHorizon")</f>
+        <f t="shared" ref="K3:K16" si="4">IF(J3="",J3,"RollingFixDispatch")</f>
         <v/>
       </c>
     </row>
@@ -5352,11 +5090,11 @@
       </c>
       <c r="J4" t="str">
         <f t="shared" si="3"/>
-        <v>30D</v>
+        <v>7D</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
+        <v>RollingFixDispatch</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -5395,11 +5133,11 @@
       </c>
       <c r="J5" t="str">
         <f t="shared" si="3"/>
-        <v>30D</v>
+        <v>7D</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
+        <v>RollingFixDispatch</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -5481,11 +5219,11 @@
       </c>
       <c r="J7" t="str">
         <f t="shared" si="3"/>
-        <v>30D</v>
+        <v>7D</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
+        <v>RollingFixDispatch</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -5524,11 +5262,11 @@
       </c>
       <c r="J8" t="str">
         <f t="shared" si="3"/>
-        <v>30D</v>
+        <v>7D</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
+        <v>RollingFixDispatch</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -5651,14 +5389,6 @@
         <f t="shared" si="2"/>
         <v>IntegerVariables</v>
       </c>
-      <c r="J11" t="str">
-        <f t="shared" si="3"/>
-        <v>30D</v>
-      </c>
-      <c r="K11" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
-      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -5687,20 +5417,12 @@
         <v>31</v>
       </c>
       <c r="H12" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="H12" si="7">IF(D12,"unit_online_variable_type_integer","")</f>
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="I12" si="8">IF(H12="",H12,"IntegerVariables")</f>
         <v>IntegerVariables</v>
-      </c>
-      <c r="J12" t="str">
-        <f t="shared" si="3"/>
-        <v>30D</v>
-      </c>
-      <c r="K12" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -5825,11 +5547,11 @@
       </c>
       <c r="J15" t="str">
         <f t="shared" si="3"/>
-        <v>30D</v>
+        <v>7D</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
+        <v>RollingFixDispatch</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -5868,11 +5590,11 @@
       </c>
       <c r="J16" t="str">
         <f t="shared" si="3"/>
-        <v>30D</v>
+        <v>7D</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
+        <v>RollingFixDispatch</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -5901,22 +5623,7 @@
       <c r="G17" t="s">
         <v>31</v>
       </c>
-      <c r="H17" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>unit_online_variable_type_integer</v>
-      </c>
-      <c r="I17" t="str">
-        <f t="shared" si="2"/>
-        <v>IntegerVariables</v>
-      </c>
-      <c r="J17" t="str">
-        <f t="shared" si="3"/>
-        <v>30D</v>
-      </c>
-      <c r="K17" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
-      </c>
+      <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -5953,12 +5660,12 @@
         <v>IntegerVariables</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" si="3"/>
-        <v>30D</v>
+        <f t="shared" ref="J18" si="9">IF(H18="unit_online_variable_type_integer","7D","")</f>
+        <v>7D</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
+        <f t="shared" ref="K18" si="10">IF(J18="",J18,"RollingFixDispatch")</f>
+        <v>RollingFixDispatch</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -5987,22 +5694,7 @@
       <c r="G19" t="s">
         <v>31</v>
       </c>
-      <c r="H19" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J19" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H19" s="7"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -6030,22 +5722,7 @@
       <c r="G20" t="s">
         <v>31</v>
       </c>
-      <c r="H20" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>unit_online_variable_type_integer</v>
-      </c>
-      <c r="I20" t="str">
-        <f t="shared" si="2"/>
-        <v>IntegerVariables</v>
-      </c>
-      <c r="J20" t="str">
-        <f t="shared" si="3"/>
-        <v>30D</v>
-      </c>
-      <c r="K20" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingHorizon</v>
-      </c>
+      <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -6078,14 +5755,6 @@
       </c>
       <c r="I21" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J21" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K21" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
add dedicated temporal blocks for thermal units
</commit_message>
<xml_diff>
--- a/model-data/all_capacities.xlsx
+++ b/model-data/all_capacities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SpineOptNordic\MESSO\model-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9F62AB-E24F-41C9-8BB5-D97BB6964DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F83CCF-607D-4C86-9BFE-173E906DFBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1BAD80D3-B61F-4294-A8B7-2B0091A5E784}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{1BAD80D3-B61F-4294-A8B7-2B0091A5E784}"/>
   </bookViews>
   <sheets>
     <sheet name="FIN" sheetId="6" r:id="rId1"/>
@@ -785,7 +785,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="80">
   <si>
     <t>Production Type</t>
   </si>
@@ -1007,6 +1007,24 @@
   </si>
   <si>
     <t>units_on_non_anticipativity_time</t>
+  </si>
+  <si>
+    <t>units_on__temporal_block</t>
+  </si>
+  <si>
+    <t>rolling_look_ahead_ST</t>
+  </si>
+  <si>
+    <t>rolling_look_ahead_ST_nuclear</t>
+  </si>
+  <si>
+    <t>false_active_alternative</t>
+  </si>
+  <si>
+    <t>active_alternative</t>
+  </si>
+  <si>
+    <t>RollingHorizon</t>
   </si>
 </sst>
 </file>
@@ -1460,10 +1478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E20367-8F61-4CFD-AF92-8269AB06E53E}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,10 +1496,12 @@
     <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1515,8 +1535,17 @@
       <c r="K1" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1550,15 +1579,24 @@
         <v>IntegerVariables</v>
       </c>
       <c r="J2" t="str">
-        <f>IF(H2="unit_online_variable_type_integer","7D","")</f>
-        <v>7D</v>
+        <f t="shared" ref="J2:J21" si="0">IF(H2="unit_online_variable_type_integer","30D","")</f>
+        <v>30D</v>
       </c>
       <c r="K2" t="str">
         <f>IF(J2="",J2,"RollingFixDispatch")</f>
         <v>RollingFixDispatch</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1570,11 +1608,11 @@
         <v>FIN_brown-coal_lignite</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D20" si="0">IF(B3&gt;0,"True","False")</f>
+        <f t="shared" ref="D3:D20" si="1">IF(B3&gt;0,"True","False")</f>
         <v>False</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E21" si="1">B3/F3</f>
+        <f t="shared" ref="E3:E21" si="2">B3/F3</f>
         <v>0</v>
       </c>
       <c r="F3">
@@ -1588,11 +1626,11 @@
         <v/>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I21" si="2">IF(H3="",H3,"IntegerVariables")</f>
+        <f t="shared" ref="I3:I21" si="3">IF(H3="",H3,"IntegerVariables")</f>
         <v/>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J16" si="3">IF(H3="unit_online_variable_type_integer","7D","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K3" t="str">
@@ -1600,7 +1638,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1612,11 +1650,11 @@
         <v>FIN_gas-coal-derived</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F4">
@@ -1630,11 +1668,11 @@
         <v/>
       </c>
       <c r="I4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K4" t="str">
@@ -1642,7 +1680,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1654,11 +1692,11 @@
         <v>FIN_gas</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>109.70588235294117</v>
       </c>
       <c r="F5">
@@ -1672,19 +1710,11 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
-      <c r="J5" t="str">
-        <f t="shared" si="3"/>
-        <v>7D</v>
-      </c>
-      <c r="K5" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingFixDispatch</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1696,11 +1726,11 @@
         <v>FIN_hard-coal</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284.75</v>
       </c>
       <c r="F6">
@@ -1714,19 +1744,28 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="3"/>
-        <v>7D</v>
+        <f t="shared" si="0"/>
+        <v>30D</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="4"/>
         <v>RollingFixDispatch</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>75</v>
+      </c>
+      <c r="M6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1738,11 +1777,11 @@
         <v>FIN_oil</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>81.529411764705884</v>
       </c>
       <c r="F7">
@@ -1756,19 +1795,11 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
-      <c r="J7" t="str">
-        <f t="shared" si="3"/>
-        <v>7D</v>
-      </c>
-      <c r="K7" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingFixDispatch</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1780,11 +1811,11 @@
         <v>FIN_oil-shale</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F8">
@@ -1798,19 +1829,11 @@
         <v/>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="K8" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1822,11 +1845,11 @@
         <v>FIN_peat</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>227</v>
       </c>
       <c r="F9">
@@ -1840,19 +1863,28 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="3"/>
-        <v>7D</v>
+        <f t="shared" si="0"/>
+        <v>30D</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="4"/>
         <v>RollingFixDispatch</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>75</v>
+      </c>
+      <c r="M9" t="s">
+        <v>37</v>
+      </c>
+      <c r="N9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1864,11 +1896,11 @@
         <v>FIN_geothermal</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F10">
@@ -1882,11 +1914,11 @@
         <v/>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K10" t="str">
@@ -1894,7 +1926,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1906,11 +1938,11 @@
         <v>FIN_hydro-pumped</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F11">
@@ -1924,11 +1956,11 @@
         <v/>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1940,11 +1972,11 @@
         <v>FIN_hydro-ror</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>64.265306122448976</v>
       </c>
       <c r="F12">
@@ -1958,11 +1990,11 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1974,11 +2006,11 @@
         <v>FIN_marine</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F13">
@@ -1992,11 +2024,11 @@
         <v/>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K13" t="str">
@@ -2004,7 +2036,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -2016,11 +2048,11 @@
         <v>FIN_nuclear</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>556.4</v>
       </c>
       <c r="F14">
@@ -2034,19 +2066,28 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="3"/>
-        <v>7D</v>
+        <f>IF(H14="unit_online_variable_type_integer","30D","")</f>
+        <v>30D</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="4"/>
         <v>RollingFixDispatch</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>76</v>
+      </c>
+      <c r="M14" t="s">
+        <v>37</v>
+      </c>
+      <c r="N14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -2058,11 +2099,11 @@
         <v>FIN_other</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>181</v>
       </c>
       <c r="F15">
@@ -2076,19 +2117,28 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="3"/>
-        <v>7D</v>
+        <f t="shared" si="0"/>
+        <v>30D</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="4"/>
         <v>RollingFixDispatch</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>75</v>
+      </c>
+      <c r="M15" t="s">
+        <v>37</v>
+      </c>
+      <c r="N15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -2100,11 +2150,11 @@
         <v>FIN_other-ren</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>257</v>
       </c>
       <c r="F16">
@@ -2118,19 +2168,28 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" si="3"/>
-        <v>7D</v>
+        <f t="shared" si="0"/>
+        <v>30D</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="4"/>
         <v>RollingFixDispatch</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>75</v>
+      </c>
+      <c r="M16" t="s">
+        <v>37</v>
+      </c>
+      <c r="N16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -2142,22 +2201,26 @@
         <v>FIN_solar</v>
       </c>
       <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>False</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="J17" t="str">
         <f t="shared" si="0"/>
-        <v>False</v>
-      </c>
-      <c r="E17" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -2169,11 +2232,11 @@
         <v>FIN_waste</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>52.333333333333336</v>
       </c>
       <c r="F18">
@@ -2187,19 +2250,28 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" ref="J18" si="6">IF(H18="unit_online_variable_type_integer","7D","")</f>
-        <v>7D</v>
+        <f t="shared" si="0"/>
+        <v>30D</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" ref="K18" si="7">IF(J18="",J18,"RollingFixDispatch")</f>
+        <f t="shared" ref="K18" si="6">IF(J18="",J18,"RollingFixDispatch")</f>
         <v>RollingFixDispatch</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>75</v>
+      </c>
+      <c r="M18" t="s">
+        <v>37</v>
+      </c>
+      <c r="N18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -2211,22 +2283,26 @@
         <v>FIN_wind-off</v>
       </c>
       <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>False</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="J19" t="str">
         <f t="shared" si="0"/>
-        <v>False</v>
-      </c>
-      <c r="E19" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -2238,7 +2314,7 @@
         <v>FIN_wind-on</v>
       </c>
       <c r="D20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E20" s="2">
@@ -2252,8 +2328,12 @@
         <v>31</v>
       </c>
       <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J20" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
@@ -2269,7 +2349,7 @@
         <v>False</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F21">
@@ -2283,18 +2363,18 @@
         <v/>
       </c>
       <c r="I21" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -2314,10 +2394,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{411AD0E3-0831-47AD-A8A3-9FE0AF10CD42}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:I12"/>
+      <selection activeCell="L2" sqref="L2:N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2332,7 +2412,7 @@
     <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2366,9 +2446,17 @@
       <c r="K1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2402,16 +2490,15 @@
         <v/>
       </c>
       <c r="J2" t="str">
-        <f>IF(H2="unit_online_variable_type_integer","7D","")</f>
+        <f t="shared" ref="J2:J21" si="0">IF(H2="unit_online_variable_type_integer","30D","")</f>
         <v/>
       </c>
       <c r="K2" t="str">
         <f>IF(J2="",J2,"RollingFixDispatch")</f>
         <v/>
       </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2423,11 +2510,11 @@
         <v>NOR_brown-coal_lignite</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D20" si="0">IF(B3&gt;0,"True","False")</f>
+        <f t="shared" ref="D3:D20" si="1">IF(B3&gt;0,"True","False")</f>
         <v>False</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E20" si="1">B3/F3</f>
+        <f t="shared" ref="E3:E20" si="2">B3/F3</f>
         <v>0</v>
       </c>
       <c r="F3">
@@ -2441,20 +2528,19 @@
         <v/>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I21" si="2">IF(H3="",H3,"IntegerVariables")</f>
+        <f t="shared" ref="I3:I21" si="3">IF(H3="",H3,"IntegerVariables")</f>
         <v/>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J16" si="3">IF(H3="unit_online_variable_type_integer","7D","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K3" t="str">
         <f t="shared" ref="K3:K16" si="4">IF(J3="",J3,"RollingFixDispatch")</f>
         <v/>
       </c>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2466,11 +2552,11 @@
         <v>NOR_gas-coal-derived</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F4">
@@ -2484,20 +2570,19 @@
         <v/>
       </c>
       <c r="I4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2509,11 +2594,11 @@
         <v>NOR_gas</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>127</v>
       </c>
       <c r="F5">
@@ -2527,20 +2612,11 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
-      <c r="J5" t="str">
-        <f t="shared" si="3"/>
-        <v>7D</v>
-      </c>
-      <c r="K5" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingFixDispatch</v>
-      </c>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -2552,11 +2628,11 @@
         <v>NOR_hard-coal</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F6">
@@ -2570,20 +2646,19 @@
         <v/>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -2595,11 +2670,11 @@
         <v>NOR_oil</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F7">
@@ -2613,20 +2688,11 @@
         <v/>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="K7" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -2638,11 +2704,11 @@
         <v>NOR_oil-shale</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F8">
@@ -2656,20 +2722,11 @@
         <v/>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="K8" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -2681,11 +2738,11 @@
         <v>NOR_peat</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F9">
@@ -2699,20 +2756,19 @@
         <v/>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -2724,11 +2780,11 @@
         <v>NOR_geothermal</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F10">
@@ -2742,20 +2798,19 @@
         <v/>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="L10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -2768,7 +2823,7 @@
         <v>NOR_hydro-pumped</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E11" s="2"/>
@@ -2777,12 +2832,11 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
-      <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -2794,11 +2848,11 @@
         <v>NOR_hydro-ror</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34.695652173913047</v>
       </c>
       <c r="F12">
@@ -2812,12 +2866,11 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
-      <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -2829,11 +2882,11 @@
         <v>NOR_marine</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F13">
@@ -2847,20 +2900,19 @@
         <v/>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -2872,11 +2924,11 @@
         <v>NOR_nuclear</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F14">
@@ -2890,20 +2942,19 @@
         <v/>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(H14="unit_online_variable_type_integer","30D","")</f>
         <v/>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -2915,11 +2966,11 @@
         <v>NOR_other</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F15">
@@ -2933,20 +2984,19 @@
         <v/>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -2958,11 +3008,11 @@
         <v>NOR_other-ren</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F16">
@@ -2976,18 +3026,17 @@
         <v/>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -3001,21 +3050,24 @@
         <v>NOR_solar</v>
       </c>
       <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>False</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="J17" t="str">
         <f t="shared" si="0"/>
-        <v>False</v>
-      </c>
-      <c r="E17" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H17" s="7"/>
-      <c r="L17" s="1"/>
+        <v/>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -3029,11 +3081,11 @@
         <v>NOR_waste</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F18">
@@ -3047,18 +3099,17 @@
         <v/>
       </c>
       <c r="I18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J18" t="str">
-        <f t="shared" ref="J18" si="6">IF(H18="unit_online_variable_type_integer","7D","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K18" t="str">
-        <f t="shared" ref="K18" si="7">IF(J18="",J18,"RollingFixDispatch")</f>
-        <v/>
-      </c>
-      <c r="L18" s="1"/>
+        <f t="shared" ref="K18" si="6">IF(J18="",J18,"RollingFixDispatch")</f>
+        <v/>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -3072,21 +3123,24 @@
         <v>NOR_wind-off</v>
       </c>
       <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>False</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="J19" t="str">
         <f t="shared" si="0"/>
-        <v>False</v>
-      </c>
-      <c r="E19" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H19" s="7"/>
-      <c r="L19" s="1"/>
+        <v/>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -3100,21 +3154,24 @@
         <v>NOR_wind-on</v>
       </c>
       <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>True</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="2"/>
+        <v>1232</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="J20" t="str">
         <f t="shared" si="0"/>
-        <v>True</v>
-      </c>
-      <c r="E20" s="2">
-        <f t="shared" si="1"/>
-        <v>1232</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H20" s="7"/>
-      <c r="L20" s="1"/>
+        <v/>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -3146,10 +3203,9 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
-      <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
@@ -3183,10 +3239,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3849322-F8A7-4330-820A-E439827D862B}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:I12"/>
+      <selection activeCell="L15" sqref="L15:N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3200,7 +3256,7 @@
     <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3234,9 +3290,17 @@
       <c r="K1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -3270,16 +3334,15 @@
         <v/>
       </c>
       <c r="J2" t="str">
-        <f>IF(H2="unit_online_variable_type_integer","7D","")</f>
+        <f t="shared" ref="J2:J21" si="0">IF(H2="unit_online_variable_type_integer","30D","")</f>
         <v/>
       </c>
       <c r="K2" t="str">
         <f>IF(J2="",J2,"RollingFixDispatch")</f>
         <v/>
       </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -3291,11 +3354,11 @@
         <v>SWE_brown-coal_lignite</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D20" si="0">IF(B3&gt;0,"True","False")</f>
+        <f t="shared" ref="D3:D20" si="1">IF(B3&gt;0,"True","False")</f>
         <v>False</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E20" si="1">B3/F3</f>
+        <f t="shared" ref="E3:E20" si="2">B3/F3</f>
         <v>0</v>
       </c>
       <c r="F3">
@@ -3309,11 +3372,11 @@
         <v/>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I21" si="2">IF(H3="",H3,"IntegerVariables")</f>
+        <f t="shared" ref="I3:I21" si="3">IF(H3="",H3,"IntegerVariables")</f>
         <v/>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J16" si="3">IF(H3="unit_online_variable_type_integer","7D","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K3" t="str">
@@ -3321,7 +3384,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -3333,11 +3396,11 @@
         <v>SWE_gas-coal-derived</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F4">
@@ -3351,11 +3414,11 @@
         <v/>
       </c>
       <c r="I4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K4" t="str">
@@ -3363,7 +3426,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3375,11 +3438,11 @@
         <v>SWE_gas</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F5">
@@ -3393,19 +3456,11 @@
         <v/>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J5" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="K5" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -3417,11 +3472,11 @@
         <v>SWE_hard-coal</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F6">
@@ -3435,11 +3490,11 @@
         <v/>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K6" t="str">
@@ -3447,7 +3502,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -3459,11 +3514,11 @@
         <v>SWE_oil</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F7">
@@ -3477,19 +3532,11 @@
         <v/>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="K7" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -3501,11 +3548,11 @@
         <v>SWE_oil-shale</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F8">
@@ -3519,19 +3566,11 @@
         <v/>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="K8" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -3543,11 +3582,11 @@
         <v>SWE_peat</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F9">
@@ -3561,11 +3600,11 @@
         <v/>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K9" t="str">
@@ -3573,7 +3612,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -3585,11 +3624,11 @@
         <v>SWE_geothermal</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8408</v>
       </c>
       <c r="F10">
@@ -3603,19 +3642,28 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="3"/>
-        <v>7D</v>
+        <f t="shared" si="0"/>
+        <v>30D</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="4"/>
         <v>RollingFixDispatch</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>75</v>
+      </c>
+      <c r="M10" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -3627,11 +3675,11 @@
         <v>SWE_hydro-pumped</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F11">
@@ -3645,11 +3693,11 @@
         <v/>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -3661,11 +3709,11 @@
         <v>SWE_hydro-ror</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F12">
@@ -3679,11 +3727,11 @@
         <v/>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -3695,11 +3743,11 @@
         <v>SWE_marine</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F13">
@@ -3713,11 +3761,11 @@
         <v/>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K13" t="str">
@@ -3725,7 +3773,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -3737,11 +3785,11 @@
         <v>SWE_nuclear</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1433.8333333333333</v>
       </c>
       <c r="F14">
@@ -3755,19 +3803,28 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="3"/>
-        <v>7D</v>
+        <f>IF(H14="unit_online_variable_type_integer","30D","")</f>
+        <v>30D</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="4"/>
         <v>RollingFixDispatch</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>76</v>
+      </c>
+      <c r="M14" t="s">
+        <v>37</v>
+      </c>
+      <c r="N14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -3779,11 +3836,11 @@
         <v>SWE_other</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F15">
@@ -3797,11 +3854,11 @@
         <v/>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K15" t="str">
@@ -3809,7 +3866,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -3821,11 +3878,11 @@
         <v>SWE_other-ren</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F16">
@@ -3839,11 +3896,11 @@
         <v/>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K16" t="str">
@@ -3863,20 +3920,24 @@
         <v>SWE_solar</v>
       </c>
       <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>True</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="J17" t="str">
         <f t="shared" si="0"/>
-        <v>True</v>
-      </c>
-      <c r="E17" s="2">
-        <f t="shared" si="1"/>
-        <v>255</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H17" s="7"/>
+        <v/>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -3890,11 +3951,11 @@
         <v>SWE_waste</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F18">
@@ -3908,15 +3969,15 @@
         <v/>
       </c>
       <c r="I18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J18" t="str">
-        <f t="shared" ref="J18" si="6">IF(H18="unit_online_variable_type_integer","7D","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K18" t="str">
-        <f t="shared" ref="K18" si="7">IF(J18="",J18,"RollingFixDispatch")</f>
+        <f t="shared" ref="K18" si="6">IF(J18="",J18,"RollingFixDispatch")</f>
         <v/>
       </c>
     </row>
@@ -3932,20 +3993,24 @@
         <v>SWE_wind-off</v>
       </c>
       <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>False</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="J19" t="str">
         <f t="shared" si="0"/>
-        <v>False</v>
-      </c>
-      <c r="E19" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H19" s="7"/>
+        <v/>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -3959,20 +4024,24 @@
         <v>SWE_wind-on</v>
       </c>
       <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>True</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="2"/>
+        <v>6247</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="J20" t="str">
         <f t="shared" si="0"/>
-        <v>True</v>
-      </c>
-      <c r="E20" s="2">
-        <f t="shared" si="1"/>
-        <v>6247</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H20" s="7"/>
+        <v/>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -4004,7 +4073,7 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
     </row>
@@ -4038,10 +4107,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E822D84-1F53-430A-8772-9025C443B1F5}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:I12"/>
+      <selection activeCell="L9" sqref="L9:N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4055,7 +4124,7 @@
     <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4089,9 +4158,17 @@
       <c r="K1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -4125,16 +4202,24 @@
         <v>IntegerVariables</v>
       </c>
       <c r="J2" t="str">
-        <f>IF(H2="unit_online_variable_type_integer","7D","")</f>
-        <v>7D</v>
+        <f t="shared" ref="J2:J21" si="0">IF(H2="unit_online_variable_type_integer","30D","")</f>
+        <v>30D</v>
       </c>
       <c r="K2" t="str">
         <f>IF(J2="",J2,"RollingFixDispatch")</f>
         <v>RollingFixDispatch</v>
       </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -4146,11 +4231,11 @@
         <v>DEN_brown-coal_lignite</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D20" si="0">IF(B3&gt;0,"True","False")</f>
+        <f t="shared" ref="D3:D20" si="1">IF(B3&gt;0,"True","False")</f>
         <v>False</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E20" si="1">B3/F3</f>
+        <f t="shared" ref="E3:E20" si="2">B3/F3</f>
         <v>0</v>
       </c>
       <c r="F3">
@@ -4164,20 +4249,19 @@
         <v/>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I21" si="2">IF(H3="",H3,"IntegerVariables")</f>
+        <f t="shared" ref="I3:I21" si="3">IF(H3="",H3,"IntegerVariables")</f>
         <v/>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J16" si="3">IF(H3="unit_online_variable_type_integer","7D","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K3" t="str">
         <f t="shared" ref="K3:K16" si="4">IF(J3="",J3,"RollingFixDispatch")</f>
         <v/>
       </c>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -4189,11 +4273,11 @@
         <v>DEN_gas-coal-derived</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F4">
@@ -4207,20 +4291,19 @@
         <v/>
       </c>
       <c r="I4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -4232,11 +4315,11 @@
         <v>DEN_gas</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>140.46153846153845</v>
       </c>
       <c r="F5">
@@ -4250,20 +4333,11 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
-      <c r="J5" t="str">
-        <f t="shared" si="3"/>
-        <v>7D</v>
-      </c>
-      <c r="K5" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingFixDispatch</v>
-      </c>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -4275,11 +4349,11 @@
         <v>DEN_hard-coal</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>609.33333333333337</v>
       </c>
       <c r="F6">
@@ -4293,20 +4367,28 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="3"/>
-        <v>7D</v>
+        <f t="shared" si="0"/>
+        <v>30D</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="4"/>
         <v>RollingFixDispatch</v>
       </c>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>75</v>
+      </c>
+      <c r="M6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -4318,11 +4400,11 @@
         <v>DEN_oil</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>335.66666666666669</v>
       </c>
       <c r="F7">
@@ -4336,20 +4418,11 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
-      <c r="J7" t="str">
-        <f t="shared" si="3"/>
-        <v>7D</v>
-      </c>
-      <c r="K7" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingFixDispatch</v>
-      </c>
-      <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -4361,11 +4434,11 @@
         <v>DEN_oil-shale</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F8">
@@ -4379,20 +4452,11 @@
         <v/>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="K8" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -4404,11 +4468,11 @@
         <v>DEN_peat</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F9">
@@ -4422,20 +4486,19 @@
         <v/>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -4447,11 +4510,11 @@
         <v>DEN_geothermal</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F10">
@@ -4465,20 +4528,19 @@
         <v/>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="L10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -4490,11 +4552,11 @@
         <v>DEN_hydro-pumped</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F11">
@@ -4508,12 +4570,11 @@
         <v/>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -4525,11 +4586,11 @@
         <v>DEN_hydro-ror</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="F12">
@@ -4543,12 +4604,11 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
-      <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -4560,11 +4620,11 @@
         <v>DEN_marine</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F13">
@@ -4578,20 +4638,19 @@
         <v/>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -4603,11 +4662,11 @@
         <v>DEN_nuclear</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F14">
@@ -4621,20 +4680,19 @@
         <v/>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(H14="unit_online_variable_type_integer","30D","")</f>
         <v/>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -4646,11 +4704,11 @@
         <v>DEN_other</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F15">
@@ -4664,20 +4722,19 @@
         <v/>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -4689,11 +4746,11 @@
         <v>DEN_other-ren</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>146</v>
       </c>
       <c r="F16">
@@ -4707,20 +4764,28 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" si="3"/>
-        <v>7D</v>
+        <f t="shared" si="0"/>
+        <v>30D</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="4"/>
         <v>RollingFixDispatch</v>
       </c>
-      <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>75</v>
+      </c>
+      <c r="M16" t="s">
+        <v>37</v>
+      </c>
+      <c r="N16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -4732,23 +4797,26 @@
         <v>DEN_solar</v>
       </c>
       <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>True</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="2"/>
+        <v>1002</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="J17" t="str">
         <f t="shared" si="0"/>
-        <v>True</v>
-      </c>
-      <c r="E17" s="2">
-        <f t="shared" si="1"/>
-        <v>1002</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H17" s="7"/>
-      <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -4760,11 +4828,11 @@
         <v>DEN_waste</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>54.857142857142854</v>
       </c>
       <c r="F18">
@@ -4778,20 +4846,28 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" ref="J18" si="6">IF(H18="unit_online_variable_type_integer","7D","")</f>
-        <v>7D</v>
+        <f t="shared" si="0"/>
+        <v>30D</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" ref="K18" si="7">IF(J18="",J18,"RollingFixDispatch")</f>
+        <f t="shared" ref="K18" si="6">IF(J18="",J18,"RollingFixDispatch")</f>
         <v>RollingFixDispatch</v>
       </c>
-      <c r="L18" s="1"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>75</v>
+      </c>
+      <c r="M18" t="s">
+        <v>37</v>
+      </c>
+      <c r="N18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -4803,23 +4879,26 @@
         <v>DEN_wind-off</v>
       </c>
       <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>True</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="2"/>
+        <v>1700</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="J19" t="str">
         <f t="shared" si="0"/>
-        <v>True</v>
-      </c>
-      <c r="E19" s="2">
-        <f t="shared" si="1"/>
-        <v>1700</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H19" s="7"/>
-      <c r="L19" s="1"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -4831,23 +4910,26 @@
         <v>DEN_wind-on</v>
       </c>
       <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>True</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="2"/>
+        <v>4423</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="J20" t="str">
         <f t="shared" si="0"/>
-        <v>True</v>
-      </c>
-      <c r="E20" s="2">
-        <f t="shared" si="1"/>
-        <v>4423</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H20" s="7"/>
-      <c r="L20" s="1"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
@@ -4877,19 +4959,18 @@
         <v/>
       </c>
       <c r="I21" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L21" s="1"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -4901,7 +4982,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="L24" s="1"/>
@@ -4914,10 +4995,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34185FE9-ED8F-4A26-B18C-A5B04A819B81}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4933,7 +5014,7 @@
     <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4967,8 +5048,17 @@
       <c r="K1" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5003,15 +5093,24 @@
         <v>IntegerVariables</v>
       </c>
       <c r="J2" t="str">
-        <f>IF(H2="unit_online_variable_type_integer","7D","")</f>
-        <v>7D</v>
+        <f t="shared" ref="J2:J21" si="0">IF(H2="unit_online_variable_type_integer","30D","")</f>
+        <v>30D</v>
       </c>
       <c r="K2" t="str">
         <f>IF(J2="",J2,"RollingFixDispatch")</f>
         <v>RollingFixDispatch</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -5024,11 +5123,11 @@
         <v>BAL_brown-coal_lignite</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D20" si="0">IF(B3&gt;0,"True","False")</f>
+        <f t="shared" ref="D3:D20" si="1">IF(B3&gt;0,"True","False")</f>
         <v>False</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E20" si="1">B3/F3</f>
+        <f t="shared" ref="E3:E20" si="2">B3/F3</f>
         <v>0</v>
       </c>
       <c r="F3">
@@ -5042,11 +5141,11 @@
         <v/>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I21" si="2">IF(H3="",H3,"IntegerVariables")</f>
+        <f t="shared" ref="I3:I21" si="3">IF(H3="",H3,"IntegerVariables")</f>
         <v/>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J16" si="3">IF(H3="unit_online_variable_type_integer","7D","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K3" t="str">
@@ -5054,7 +5153,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -5067,11 +5166,11 @@
         <v>BAL_gas-coal-derived</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
       <c r="F4">
@@ -5085,19 +5184,28 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
       <c r="J4" t="str">
-        <f t="shared" si="3"/>
-        <v>7D</v>
+        <f t="shared" si="0"/>
+        <v>30D</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="4"/>
         <v>RollingFixDispatch</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>75</v>
+      </c>
+      <c r="M4" t="s">
+        <v>37</v>
+      </c>
+      <c r="N4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -5110,11 +5218,11 @@
         <v>BAL_gas</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>311.60000000000002</v>
       </c>
       <c r="F5">
@@ -5128,19 +5236,11 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
-      <c r="J5" t="str">
-        <f t="shared" si="3"/>
-        <v>7D</v>
-      </c>
-      <c r="K5" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingFixDispatch</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -5153,11 +5253,11 @@
         <v>BAL_hard-coal</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F6">
@@ -5171,11 +5271,11 @@
         <v/>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K6" t="str">
@@ -5183,7 +5283,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -5196,11 +5296,11 @@
         <v>BAL_oil</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="F7">
@@ -5214,19 +5314,11 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
-      <c r="J7" t="str">
-        <f t="shared" si="3"/>
-        <v>7D</v>
-      </c>
-      <c r="K7" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingFixDispatch</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -5239,11 +5331,11 @@
         <v>BAL_oil-shale</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>658.66666666666663</v>
       </c>
       <c r="F8">
@@ -5257,19 +5349,11 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
-      <c r="J8" t="str">
-        <f t="shared" si="3"/>
-        <v>7D</v>
-      </c>
-      <c r="K8" t="str">
-        <f t="shared" si="4"/>
-        <v>RollingFixDispatch</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -5282,11 +5366,11 @@
         <v>BAL_peat</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F9">
@@ -5300,11 +5384,11 @@
         <v/>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K9" t="str">
@@ -5312,7 +5396,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -5325,11 +5409,11 @@
         <v>BAL_geothermal</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F10">
@@ -5343,11 +5427,11 @@
         <v/>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K10" t="str">
@@ -5355,7 +5439,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -5368,11 +5452,11 @@
         <v>BAL_hydro-pumped</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>225</v>
       </c>
       <c r="F11">
@@ -5386,11 +5470,11 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -5403,11 +5487,11 @@
         <v>BAL_hydro-ror</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>335</v>
       </c>
       <c r="F12">
@@ -5425,7 +5509,7 @@
         <v>IntegerVariables</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -5438,11 +5522,11 @@
         <v>BAL_marine</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F13">
@@ -5456,11 +5540,11 @@
         <v/>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K13" t="str">
@@ -5468,7 +5552,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -5481,11 +5565,11 @@
         <v>BAL_nuclear</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>False</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F14">
@@ -5499,11 +5583,11 @@
         <v/>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(H14="unit_online_variable_type_integer","30D","")</f>
         <v/>
       </c>
       <c r="K14" t="str">
@@ -5511,7 +5595,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -5524,11 +5608,11 @@
         <v>BAL_other</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18.5</v>
       </c>
       <c r="F15">
@@ -5542,19 +5626,28 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="3"/>
-        <v>7D</v>
+        <f t="shared" si="0"/>
+        <v>30D</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="4"/>
         <v>RollingFixDispatch</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>75</v>
+      </c>
+      <c r="M15" t="s">
+        <v>37</v>
+      </c>
+      <c r="N15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -5567,11 +5660,11 @@
         <v>BAL_other-ren</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="F16">
@@ -5585,19 +5678,28 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" si="3"/>
-        <v>7D</v>
+        <f t="shared" si="0"/>
+        <v>30D</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="4"/>
         <v>RollingFixDispatch</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>75</v>
+      </c>
+      <c r="M16" t="s">
+        <v>37</v>
+      </c>
+      <c r="N16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -5610,22 +5712,26 @@
         <v>BAL_solar</v>
       </c>
       <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>True</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="2"/>
+        <v>83</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="J17" t="str">
         <f t="shared" si="0"/>
-        <v>True</v>
-      </c>
-      <c r="E17" s="2">
-        <f t="shared" si="1"/>
-        <v>83</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -5638,11 +5744,11 @@
         <v>BAL_waste</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>True</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.666666666666666</v>
       </c>
       <c r="F18">
@@ -5656,19 +5762,28 @@
         <v>unit_online_variable_type_integer</v>
       </c>
       <c r="I18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>IntegerVariables</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" ref="J18" si="9">IF(H18="unit_online_variable_type_integer","7D","")</f>
-        <v>7D</v>
+        <f t="shared" si="0"/>
+        <v>30D</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" ref="K18" si="10">IF(J18="",J18,"RollingFixDispatch")</f>
+        <f t="shared" ref="K18" si="9">IF(J18="",J18,"RollingFixDispatch")</f>
         <v>RollingFixDispatch</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>75</v>
+      </c>
+      <c r="M18" t="s">
+        <v>37</v>
+      </c>
+      <c r="N18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -5681,22 +5796,26 @@
         <v>BAL_wind-off</v>
       </c>
       <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>False</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="J19" t="str">
         <f t="shared" si="0"/>
-        <v>False</v>
-      </c>
-      <c r="E19" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -5709,22 +5828,26 @@
         <v>BAL_wind-on</v>
       </c>
       <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>True</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="2"/>
+        <v>1049</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="J20" t="str">
         <f t="shared" si="0"/>
-        <v>True</v>
-      </c>
-      <c r="E20" s="2">
-        <f t="shared" si="1"/>
-        <v>1049</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
@@ -5754,18 +5877,18 @@
         <v/>
       </c>
       <c r="I21" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>

</xml_diff>